<commit_message>
changing class names for customer care module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -49,18 +49,12 @@
     <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported||Ensure that the page has "Support Request" and "Call us" sections.</t>
   </si>
   <si>
-    <t>DRAIAMCC004</t>
-  </si>
-  <si>
     <t>OPQA-5229||OPQA-5230</t>
   </si>
   <si>
     <t>Verify that Page should change header title for different title||Ensure that the page has "Support Request" and "Call us" sections.</t>
   </si>
   <si>
-    <t>DRAIAMCC003</t>
-  </si>
-  <si>
     <t>OPQA-5174</t>
   </si>
   <si>
@@ -79,12 +73,6 @@
     <t>Verify that error messages/validation alerts " Incorrect email address format. Please try again." should be displayed when user enters incorrect email address.||Verify that error messages/validation alerts "Incorrect phone number format. Please try again.." should be displayed when user enters incorrect phone number.</t>
   </si>
   <si>
-    <t>DRAIAMCC001</t>
-  </si>
-  <si>
-    <t>DRAIAMCC002</t>
-  </si>
-  <si>
     <t>OPQA-5155</t>
   </si>
   <si>
@@ -97,21 +85,9 @@
     <t>Verify that the page shall be accessible in both an authenticated and a non-authenticated state</t>
   </si>
   <si>
-    <t>IPAIAMCC001</t>
-  </si>
-  <si>
-    <t>IPAIAMCC002</t>
-  </si>
-  <si>
-    <t>IPAIAMCC003</t>
-  </si>
-  <si>
     <t>Verify that the user should be able to select the issue type/category of the issue as an option</t>
   </si>
   <si>
-    <t>IPAIAMCC004</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -121,23 +97,47 @@
     <t>IPAIAMCC071</t>
   </si>
   <si>
-    <t>DRAIAMCC070</t>
-  </si>
-  <si>
-    <t>DRAIAMCC071</t>
-  </si>
-  <si>
-    <t>DRAIAMCC072</t>
-  </si>
-  <si>
-    <t>DRAIAMCC073</t>
+    <t>Customercare001</t>
+  </si>
+  <si>
+    <t>Customercare002</t>
+  </si>
+  <si>
+    <t>Customercare003</t>
+  </si>
+  <si>
+    <t>Customercare004</t>
+  </si>
+  <si>
+    <t>Customercare005</t>
+  </si>
+  <si>
+    <t>Customercare006</t>
+  </si>
+  <si>
+    <t>Customercare007</t>
+  </si>
+  <si>
+    <t>Customercare008</t>
+  </si>
+  <si>
+    <t>Customercare009</t>
+  </si>
+  <si>
+    <t>Customercare010</t>
+  </si>
+  <si>
+    <t>Customercare011</t>
+  </si>
+  <si>
+    <t>Customercare012</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,7 +327,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -359,10 +359,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,7 +393,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -570,23 +568,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,9 +601,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
@@ -618,9 +616,9 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75">
       <c r="A3" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -633,162 +631,162 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="45">
       <c r="A9" s="6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="45">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="45">
+      <c r="A11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>12</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>8</v>
@@ -797,13 +795,13 @@
         <v>9</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="75">
       <c r="A15" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
@@ -812,165 +810,165 @@
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
       <c r="D16" s="11"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
       <c r="D17" s="11"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="D18" s="11"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="6"/>
       <c r="B19" s="3"/>
       <c r="C19" s="7"/>
       <c r="D19" s="11"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="12"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="12"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="12"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="12"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30.75" customHeight="1">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="2"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="2"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="2"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="2"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="2"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="3"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="3"/>

</xml_diff>

<commit_message>
class name changes for customer care testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -91,12 +91,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>IPAIAMCC070</t>
-  </si>
-  <si>
-    <t>IPAIAMCC071</t>
-  </si>
-  <si>
     <t>Customercare001</t>
   </si>
   <si>
@@ -131,6 +125,12 @@
   </si>
   <si>
     <t>Customercare012</t>
+  </si>
+  <si>
+    <t>Customercare013</t>
+  </si>
+  <si>
+    <t>Customercare014</t>
   </si>
 </sst>
 </file>
@@ -572,7 +572,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -603,7 +603,7 @@
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="3" spans="1:6" ht="75">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="4" spans="1:6" ht="30">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>18</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>19</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>10</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>12</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="8" spans="1:6" ht="45">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>14</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="9" spans="1:6" ht="45">
       <c r="A9" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>16</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="10" spans="1:6" ht="45">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>14</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="11" spans="1:6" ht="45">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>16</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>10</v>
@@ -785,8 +785,8 @@
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="30">
-      <c r="A14" s="6" t="s">
-        <v>24</v>
+      <c r="A14" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>8</v>
@@ -800,8 +800,8 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="75">
-      <c r="A15" s="6" t="s">
-        <v>25</v>
+      <c r="A15" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added in new customer care script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>TCID</t>
   </si>
@@ -132,12 +132,21 @@
   <si>
     <t>Customercare014</t>
   </si>
+  <si>
+    <t>Customercare015</t>
+  </si>
+  <si>
+    <t>OPQA-5320||OPQA-5321||OPQA5322||OPQA-5323</t>
+  </si>
+  <si>
+    <t>verify that upon clicking on submit button, a success message should be displayed that confirms submission and should allow user to raise a new ticket||Verify that success message in customer care page should match with wire frame||verify that extension field should be placed next to phone number field in customer care page||Verify that all characters including special characters should be allowed in extension field in customer care page.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,6 +368,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -393,6 +403,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -568,23 +579,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
@@ -616,7 +627,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="75">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -631,7 +642,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
@@ -646,7 +657,7 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
@@ -661,7 +672,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>31</v>
       </c>
@@ -676,7 +687,7 @@
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -691,7 +702,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
@@ -706,7 +717,7 @@
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="45">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
@@ -721,7 +732,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="45">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -736,7 +747,7 @@
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -752,7 +763,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
@@ -768,7 +779,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
@@ -784,7 +795,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="30">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -799,7 +810,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="75">
+    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -814,161 +825,169 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="11"/>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
       <c r="D17" s="11"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="D18" s="11"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="3"/>
       <c r="C19" s="7"/>
       <c r="D19" s="11"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="12"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="12"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="12"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="12"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" ht="30.75" customHeight="1">
+    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="2"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="2"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="2"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="2"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="2"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="3"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="3"/>

</xml_diff>

<commit_message>
Added new Customer care script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>verify that upon clicking on submit button, a success message should be displayed that confirms submission and should allow user to raise a new ticket||Verify that success message in customer care page should match with wire frame||verify that extension field should be placed next to phone number field in customer care page||Verify that all characters including special characters should be allowed in extension field in customer care page.</t>
+  </si>
+  <si>
+    <t>Customercare016</t>
+  </si>
+  <si>
+    <t>OPQA-5191||OPQA-5194||OPQA-5196||OPQA-5197</t>
+  </si>
+  <si>
+    <t>Verify that the text "Drug Research Advisor Customer Care " should be hyperlinked and it should be linked to customer care / support page.||Verify that 'DRA_support@thomsonreuters.com' is replaced with ' Drug Research Advisor Customer Care.'||Verify that hyperlinked text "Drug Research Advisor Customer Care " should be opened in a second window / tab (based on user/browser preference)||Verify that the customer care page URL content shall be specific to DRA(Target Druggability)</t>
   </si>
 </sst>
 </file>
@@ -230,9 +239,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -246,6 +252,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,7 +592,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +614,7 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -613,217 +622,217 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -832,167 +841,175 @@
       <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="11"/>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="12"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="12"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="6"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="6"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="6"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="6"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="6"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new cc script for opqa-5173
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6360"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>TCID</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Verify that the text "Drug Research Advisor Customer Care " should be hyperlinked and it should be linked to customer care / support page.||Verify that 'DRA_support@thomsonreuters.com' is replaced with ' Drug Research Advisor Customer Care.'||Verify that hyperlinked text "Drug Research Advisor Customer Care " should be opened in a second window / tab (based on user/browser preference)||Verify that the customer care page URL content shall be specific to DRA(Target Druggability)</t>
+  </si>
+  <si>
+    <t>Customercare020</t>
+  </si>
+  <si>
+    <t>OPQA-5173</t>
+  </si>
+  <si>
+    <t>Verify that If the user is logged-in into the application, The system should prefill the webform with the name, contact information, organization, and country information obtained from the user's STeAM account</t>
   </si>
 </sst>
 </file>
@@ -345,7 +354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,7 +389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -864,11 +873,19 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="10"/>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New developed and ENW fixed scripts have been committed
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6360"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>TCID</t>
   </si>
@@ -158,6 +158,19 @@
   </si>
   <si>
     <t>Verify that If the user is logged-in into the application, The system should prefill the webform with the name, contact information, organization, and country information obtained from the user's STeAM account</t>
+  </si>
+  <si>
+    <t>Customercare021</t>
+  </si>
+  <si>
+    <t>OPQA-5298 
+||OPQA-5299
+|| OPQA-5300</t>
+  </si>
+  <si>
+    <t>Verify that Phone Number format should Only allow digits, ‘+’ sign (at beginning), dashes ‘-‘, parentheses '()' and spaces within the field
+Verify that spaces and special characters should be stripped out from the phone Number field before being submitted to salesforce
+Verify that Minimum 7 digits and Maximum of 40 characters should be inputted in the phone field in customer care page</t>
   </si>
 </sst>
 </file>
@@ -354,7 +367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,7 +402,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,13 +613,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="29" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
@@ -888,11 +901,19 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="10"/>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new customercare script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6360"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>TCID</t>
   </si>
@@ -171,6 +171,15 @@
     <t>Verify that Phone Number format should Only allow digits, ‘+’ sign (at beginning), dashes ‘-‘, parentheses '()' and spaces within the field
 Verify that spaces and special characters should be stripped out from the phone Number field before being submitted to salesforce
 Verify that Minimum 7 digits and Maximum of 40 characters should be inputted in the phone field in customer care page</t>
+  </si>
+  <si>
+    <t>Verify that Countries list should be updated to match with SFDC list in customer care page as per document OPWLRA-630.xlsx.</t>
+  </si>
+  <si>
+    <t>OPQA-5350</t>
+  </si>
+  <si>
+    <t>Customercare017</t>
   </si>
 </sst>
 </file>
@@ -614,7 +623,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,11 +926,19 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>

</xml_diff>

<commit_message>
Blocked IPA customercare script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6360"/>
@@ -385,7 +385,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,7 +420,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +762,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E8" s="5"/>
     </row>

</xml_diff>

<commit_message>
added OPQA-5196/OPQA-5191 to cc001
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6360"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -179,17 +179,17 @@
     <t>Verify that the user is able to manually select any particular country and see contact details associated with it as per Neon Local support numbers v2.doc||Verify that toll free numbers are getting displayed as per wireframes.</t>
   </si>
   <si>
-    <t>OPQA-5154||OPQA-5230||OPQA-5354</t>
-  </si>
-  <si>
-    <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported||Ensure that the page has "Support Request" and "Call us" sections.||Verify that icons are added to phone,timing and language.</t>
+    <t>OPQA-5154||OPQA-5230||OPQA-5354||OPQA-5196||OPQA-5191</t>
+  </si>
+  <si>
+    <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported||Ensure that the page has "Support Request" and "Call us" sections.||Verify that icons are added to phone,timing and language.||Verify that hyperlinked text "Drug Research Advisor Customer Care " should be opened in a second window / tab (based on user/browser preference)||Verify that the text "Drug Research Advisor Customer Care " should be hyperlinked and it should be linked to customer care / support page.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,7 +379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,10 +411,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,7 +445,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -622,14 +620,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="29" customWidth="1" collapsed="1"/>
@@ -638,7 +636,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,7 +653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="51.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -670,7 +668,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -685,7 +683,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -700,7 +698,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -715,7 +713,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -730,7 +728,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -745,7 +743,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -760,7 +758,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="45">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -776,7 +774,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -792,7 +790,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -808,7 +806,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
@@ -823,7 +821,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="75">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -838,7 +836,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
@@ -853,7 +851,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="60">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -868,7 +866,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -883,7 +881,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="45">
       <c r="A17" s="5" t="s">
         <v>41</v>
       </c>
@@ -898,7 +896,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
@@ -913,7 +911,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
         <v>47</v>
       </c>
@@ -928,119 +926,119 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="11"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="7"/>
       <c r="D21" s="11"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="30.75" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="D26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
       <c r="D32" s="2"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
       <c r="D33" s="2"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="D34" s="2"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="3"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="3"/>

</xml_diff>

<commit_message>
Replace Thread.Sleep() method to Explicit wait in IPAIAM module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/customercare.xlsx
+++ b/src/test/resources/xls/customercare.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18975" windowHeight="5025"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>TCID</t>
   </si>
@@ -76,9 +77,6 @@
     <t>Verify that the user should be able to select the issue type/category of the issue as an option</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Customercare001</t>
   </si>
   <si>
@@ -194,8 +192,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -288,7 +286,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,7 +382,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -417,9 +414,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,6 +449,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -626,14 +625,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C19:C20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="29" customWidth="1" collapsed="1"/>
@@ -642,7 +641,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,24 +658,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="127.5" customHeight="1">
+    <row r="2" spans="1:6" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="75">
-      <c r="A3" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
@@ -689,24 +688,24 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>16</v>
@@ -719,24 +718,24 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="30">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>12</v>
@@ -749,9 +748,9 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>14</v>
@@ -764,9 +763,9 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="45">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>14</v>
@@ -775,46 +774,46 @@
         <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="30">
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
@@ -823,13 +822,13 @@
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="75">
+    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>6</v>
@@ -838,213 +837,213 @@
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="D14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" ht="60">
-      <c r="A15" s="3" t="s">
+      <c r="B15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="D15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="45">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="45">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="5" t="s">
+      <c r="D18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="11"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="11"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="30.75" customHeight="1">
+    <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="D26" s="2"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
       <c r="D32" s="2"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
       <c r="D33" s="2"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="D34" s="2"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="3"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="3"/>

</xml_diff>